<commit_message>
Izveidots testēšanas apraksts un prasības
</commit_message>
<xml_diff>
--- a/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
+++ b/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Tests_Bardulis</t>
   </si>
@@ -45,9 +45,6 @@
     <t>AIZ</t>
   </si>
   <si>
-    <t>JAU</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Nepareiza atbilde</t>
   </si>
   <si>
-    <t>Jautājums</t>
-  </si>
-  <si>
     <t>Rezultatu izvade</t>
   </si>
   <si>
@@ -102,25 +96,232 @@
     <t>Sākums</t>
   </si>
   <si>
-    <t>Prgrammas "Tests" aizvēršana</t>
-  </si>
-  <si>
-    <t>Jautājumi un atbildes</t>
-  </si>
-  <si>
     <t>PR.AIZ.01.</t>
+  </si>
+  <si>
+    <t>PR.PA.01.</t>
+  </si>
+  <si>
+    <t>PR.PA.02.</t>
+  </si>
+  <si>
+    <t>PR.NA.02.</t>
+  </si>
+  <si>
+    <t>PR.PA.03.</t>
+  </si>
+  <si>
+    <t>PR.NA.03.</t>
+  </si>
+  <si>
+    <t>PR.PA.04.</t>
+  </si>
+  <si>
+    <t>PR.NA.04.</t>
+  </si>
+  <si>
+    <t>PR.PA.05.</t>
+  </si>
+  <si>
+    <t>PR.NA.05.</t>
+  </si>
+  <si>
+    <t>PR.PA.06.</t>
+  </si>
+  <si>
+    <t>PR.NA.06.</t>
+  </si>
+  <si>
+    <t>PR.PA.07.</t>
+  </si>
+  <si>
+    <t>PR.NA.07.</t>
+  </si>
+  <si>
+    <t>PR.NA.08.</t>
+  </si>
+  <si>
+    <t>PR.PA.08.</t>
+  </si>
+  <si>
+    <t>PR.PA.09.</t>
+  </si>
+  <si>
+    <t>PR.NA.09</t>
+  </si>
+  <si>
+    <r>
+      <t>PR.PA.10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="186"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>PR.NA.10.</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>Gara atbilde</t>
+  </si>
+  <si>
+    <t>PR.GA.01.</t>
+  </si>
+  <si>
+    <t>PR.NA.01.</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Tukša atbilde</t>
+  </si>
+  <si>
+    <t>PR.TA.01.</t>
+  </si>
+  <si>
+    <t>Rezultātu izvade</t>
+  </si>
+  <si>
+    <t>1. jautājums</t>
+  </si>
+  <si>
+    <t>2. jautājums</t>
+  </si>
+  <si>
+    <t>3. jautājums</t>
+  </si>
+  <si>
+    <t>4. jautājums</t>
+  </si>
+  <si>
+    <t>5. jautājums</t>
+  </si>
+  <si>
+    <t>6. jautājums</t>
+  </si>
+  <si>
+    <t>7. jautājums</t>
+  </si>
+  <si>
+    <t>8. jautājums</t>
+  </si>
+  <si>
+    <t>9. jautājums</t>
+  </si>
+  <si>
+    <t>10. jautājums</t>
+  </si>
+  <si>
+    <t>PR.REZ.02.</t>
+  </si>
+  <si>
+    <t>PR.REZ.01.</t>
+  </si>
+  <si>
+    <t>Izvada jautājumus uz kuriem atbildēts nepareizi.</t>
+  </si>
+  <si>
+    <t>Izvada pareizi atbildēto jautājumu skaitu.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 10. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 10. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 9. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 9. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 8. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 8. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 7. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 7. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 6. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 6. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 5. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 5. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 4. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 4. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 3. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 3. jautājumam.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 2. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 2. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pārāk garas atbildes uzskatīšanu par nepareizu atbildi.</t>
+  </si>
+  <si>
+    <t>Neuzdod nākamo jautājumu kamēr nav atbildēts uz nākamo jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareizas atbildes reģistrācija 1. jautājumam.</t>
+  </si>
+  <si>
+    <t>Pareizas atbildes reģistrācija 1. jautājumam.</t>
+  </si>
+  <si>
+    <t>Programmas "Tests" aizvēršana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -181,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -230,43 +431,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,148 +768,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="B6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+  <mergeCells count="14">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -699,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A26" sqref="A26:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,149 +941,316 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>23</v>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>26</v>
+      <c r="A5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="15"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
+      <c r="A26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="15"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="15"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="17"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="13">
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Veikta testēšanas žurnāla testpiemēru izstrāde
</commit_message>
<xml_diff>
--- a/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
+++ b/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="221">
   <si>
     <t>Tests_Bardulis</t>
   </si>
@@ -303,17 +303,440 @@
   <si>
     <t>Programmas "Tests" aizvēršana</t>
   </si>
+  <si>
+    <t>Testpiemēra ID</t>
+  </si>
+  <si>
+    <t>Testpiemēra nosaukums</t>
+  </si>
+  <si>
+    <t>Testpiemēra apraksts</t>
+  </si>
+  <si>
+    <t>Testpiemēra izpildes soļi</t>
+  </si>
+  <si>
+    <t>Testpiemēra ievades dati</t>
+  </si>
+  <si>
+    <t>Testpiemēra izpildes sagaidāmais rezultāts</t>
+  </si>
+  <si>
+    <t>Prasību identifikators</t>
+  </si>
+  <si>
+    <t>Black Box</t>
+  </si>
+  <si>
+    <t>TP.STA.01.</t>
+  </si>
+  <si>
+    <t>Programmas startēšana</t>
+  </si>
+  <si>
+    <t>Uz Windows darbastacijas uzstādīta programma "Tests".</t>
+  </si>
+  <si>
+    <t>Programmas palaišana uz Windows darbstacijas</t>
+  </si>
+  <si>
+    <t>1) Uz Windows darbstacijas uzstāda programmu
+2) Peles kreisā taustiņa dubultklikšķis uz Tests.exe saīsnes.</t>
+  </si>
+  <si>
+    <t>Peles kreisā taustiņa dubultklikšķis</t>
+  </si>
+  <si>
+    <t>Tiek startēta programma "Tests"</t>
+  </si>
+  <si>
+    <t>TP.AIZ.01.</t>
+  </si>
+  <si>
+    <t>Programmas apturēšana</t>
+  </si>
+  <si>
+    <t>Jābūt startātai programai "Tests".</t>
+  </si>
+  <si>
+    <t>Uz Windows darbastacijas startētās programmas "Tests" apturēšana.</t>
+  </si>
+  <si>
+    <t>Peles kreisā taustiņa klikšķis</t>
+  </si>
+  <si>
+    <t>1) Peles kreisais klikšķis uz pogas programmas loga augšējā labā stūrī ar apzīmējumu "X"</t>
+  </si>
+  <si>
+    <t>Tiek apturēta programma "Tests"</t>
+  </si>
+  <si>
+    <t>TP.PA.01.</t>
+  </si>
+  <si>
+    <t>TP.NA.01.</t>
+  </si>
+  <si>
+    <t>TP.GA.01.</t>
+  </si>
+  <si>
+    <t>TP.TA.01.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 1. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 1. jautājumu.</t>
+  </si>
+  <si>
+    <t>Tukša atbilde uz jautājumu</t>
+  </si>
+  <si>
+    <t>Pārāk gara atbilde uz jautājumu</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 1. jautājumam.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 1. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 1. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta tukša atbilde.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pārāk gara atbilde uz jautājumu.</t>
+  </si>
+  <si>
+    <t>Testpiemēra izpildes nosacījumi</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts teksts "tests"
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Piespiež ENTER taustiņu.</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "A" 
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "C".
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķis, taustiņš "A" un taustiņš ENTER.</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķis, taustiņš "C" un taustiņš ENTER.</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķis, teksts "tests" un taustiņš ENTER.</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķi un taustiņš ENTER..</t>
+  </si>
+  <si>
+    <t>Programmas beigās paziņo, ka atbilde ir pareiza.</t>
+  </si>
+  <si>
+    <t>Programmas beigās paziņo, ka atbilde ir nepareiza.</t>
+  </si>
+  <si>
+    <t>Programma liek vēlreiz ievadīt atbildi.</t>
+  </si>
+  <si>
+    <t>TP.PA.02.</t>
+  </si>
+  <si>
+    <t>TP.NA.02.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 2. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 2. jautājumu.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 2. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 2. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 2. jautājumu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "B" 
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "A".
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķis, taustiņš "B" un taustiņš ENTER.</t>
+  </si>
+  <si>
+    <t>TP.PA.03.</t>
+  </si>
+  <si>
+    <t>TP.NA.03.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 3. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 3. jautājumu.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 3. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 3. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 3. jautājumu</t>
+  </si>
+  <si>
+    <t>TP.PA.04.</t>
+  </si>
+  <si>
+    <t>TP.NA.04.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 4. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 4. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 4. jautājumu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "D".
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>Peles kreisais klikšķis, taustiņš "D" un taustiņš ENTER.</t>
+  </si>
+  <si>
+    <t>PR.NA.09.</t>
+  </si>
+  <si>
+    <t>PR.PA.10.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 10. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 10. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 9. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 9. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 8. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 8. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 7. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 7. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 6. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 6. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 5. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 5. jautājumu.</t>
+  </si>
+  <si>
+    <t>Nepareiza atbilde uz 4. jautājumu.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 4. jautājumu.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 5. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 5. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 5. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 6. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 6. jautājumu</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 6. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 7. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 7. jautājumu</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 7. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 8. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 8. jautājumu</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 8. jautājumam.</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 9. jautājumam.</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 9. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 9. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta pareizā atbilde uz 10. jautājumu</t>
+  </si>
+  <si>
+    <t>Tiek ievadīta un reģistrēta nepareizā atbilde uz 10. jautājumu</t>
+  </si>
+  <si>
+    <t>Jabūt startētai programmai un atvērtam 10. jautājumam.</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "B".
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>1) startē programmu "Tests" 
+2) Tiek ievadīts burts "C" 
+3) Apsiprina atbildi piespiežot ENTER taustiņu</t>
+  </si>
+  <si>
+    <t>TP.PA.05.</t>
+  </si>
+  <si>
+    <t>TP.NA.05.</t>
+  </si>
+  <si>
+    <t>TP.PA.06.</t>
+  </si>
+  <si>
+    <t>TP.NA.06.</t>
+  </si>
+  <si>
+    <t>TP.NA.07.</t>
+  </si>
+  <si>
+    <t>TP.PA.07.</t>
+  </si>
+  <si>
+    <t>TP.PA.08.</t>
+  </si>
+  <si>
+    <t>TP.NA.08.</t>
+  </si>
+  <si>
+    <t>TP.NA.09.</t>
+  </si>
+  <si>
+    <t>TP.PA.09.</t>
+  </si>
+  <si>
+    <t>TP.PA.10.</t>
+  </si>
+  <si>
+    <t>TP.NA.10.</t>
+  </si>
+  <si>
+    <t>TP.REZ.01.</t>
+  </si>
+  <si>
+    <t>TP.REZ.02.</t>
+  </si>
+  <si>
+    <t>Izvada rezultātu par pareizām atbildēm</t>
+  </si>
+  <si>
+    <t>Izvada rezultātu par nepareizām atbildēm</t>
+  </si>
+  <si>
+    <t>Jāatbild uz visiem 10 jautājumiem.</t>
+  </si>
+  <si>
+    <t>Tiek izvadīts paziņojums par pareizi atbildēto jautājumu skaitu.</t>
+  </si>
+  <si>
+    <t>Tiek izvadīts paziņojums ar nepareizi atbildētiem jautājumiem.</t>
+  </si>
+  <si>
+    <t>1) Startē programmu "Tests" 
+2) Atbild uz visiem 10 jautājumiem</t>
+  </si>
+  <si>
+    <t>Taustiņi "A", "B", "C", "D" un ENTER .</t>
+  </si>
+  <si>
+    <t>Paziņojumā izvada sarakstu ar nepareizi atbildētiem jautājumiem.</t>
+  </si>
+  <si>
+    <t>Paziņojumā izvada skaitu uz cik jautājumiem atbildēts pareizi.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -361,8 +784,17 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +810,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,49 +882,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,16 +1236,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
@@ -798,7 +1254,7 @@
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10"/>
@@ -825,57 +1281,57 @@
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -890,7 +1346,7 @@
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="10"/>
@@ -899,7 +1355,7 @@
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="10"/>
@@ -930,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:B26"/>
     </sheetView>
   </sheetViews>
@@ -961,10 +1417,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -975,10 +1431,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -1013,10 +1469,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="17"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1035,10 +1491,10 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1057,10 +1513,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -1079,10 +1535,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -1101,10 +1557,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
@@ -1123,10 +1579,10 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="17"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
@@ -1145,10 +1601,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="17"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -1167,10 +1623,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="17"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1189,10 +1645,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="17"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
@@ -1211,10 +1667,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="18"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
@@ -1233,11 +1689,14 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A38:B38"/>
@@ -1248,9 +1707,6 @@
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1258,13 +1714,887 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+    </row>
+    <row r="27" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+    </row>
+    <row r="33" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A17:H17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Izveidots README.md un pievienots mācību materiāls
</commit_message>
<xml_diff>
--- a/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
+++ b/Testesanas_dokumentacijas_Bardulis_2PT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Apraksts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="259">
   <si>
     <t>Tests_Bardulis</t>
   </si>
@@ -718,12 +718,126 @@
   <si>
     <t>Paziņojumā izvada skaitu uz cik jautājumiem atbildēts pareizi.</t>
   </si>
+  <si>
+    <t>Testēšanas  ID</t>
+  </si>
+  <si>
+    <t>Datums</t>
+  </si>
+  <si>
+    <t>Testētājs</t>
+  </si>
+  <si>
+    <t>Statuss</t>
+  </si>
+  <si>
+    <t>Kļūdas paziņojums</t>
+  </si>
+  <si>
+    <t>Kļūdas paziņojuma Nr.</t>
+  </si>
+  <si>
+    <t>18.06.2021.</t>
+  </si>
+  <si>
+    <t>TZ.01.</t>
+  </si>
+  <si>
+    <t>TZ.02.</t>
+  </si>
+  <si>
+    <t>Mārtiņš Bardulis</t>
+  </si>
+  <si>
+    <t>Veiksmīgs</t>
+  </si>
+  <si>
+    <t>TZ.05.</t>
+  </si>
+  <si>
+    <t>TZ.04.</t>
+  </si>
+  <si>
+    <t>TZ.03.</t>
+  </si>
+  <si>
+    <t>TZ.06.</t>
+  </si>
+  <si>
+    <t>TZ.07.</t>
+  </si>
+  <si>
+    <t>TZ.08.</t>
+  </si>
+  <si>
+    <t>TZ.09.</t>
+  </si>
+  <si>
+    <t>TZ.10.</t>
+  </si>
+  <si>
+    <t>TZ.11.</t>
+  </si>
+  <si>
+    <t>TZ.12</t>
+  </si>
+  <si>
+    <t>TZ.13.</t>
+  </si>
+  <si>
+    <t>TZ.14.</t>
+  </si>
+  <si>
+    <t>TZ.15.</t>
+  </si>
+  <si>
+    <t>TZ.16.</t>
+  </si>
+  <si>
+    <t>TZ.17.</t>
+  </si>
+  <si>
+    <t>TZ.18.</t>
+  </si>
+  <si>
+    <t>TZ.19.</t>
+  </si>
+  <si>
+    <t>TZ.20.</t>
+  </si>
+  <si>
+    <t>TZ.21.</t>
+  </si>
+  <si>
+    <t>TZ.22.</t>
+  </si>
+  <si>
+    <t>TZ.23.</t>
+  </si>
+  <si>
+    <t>TZ.24.</t>
+  </si>
+  <si>
+    <t>Pareiza atbilde uz 2 jautājumu.</t>
+  </si>
+  <si>
+    <t>TZ.25.</t>
+  </si>
+  <si>
+    <t>TZ.26.</t>
+  </si>
+  <si>
+    <t>TZ.27.</t>
+  </si>
+  <si>
+    <t>TZ.28.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,6 +907,30 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -820,7 +958,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -878,11 +1016,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -893,6 +1042,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -914,36 +1072,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Parasts" xfId="0" builtinId="0"/>
@@ -1236,129 +1417,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1417,10 +1598,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
@@ -1431,10 +1612,10 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -1469,10 +1650,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="19"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -1491,10 +1672,10 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -1513,10 +1694,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="19"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -1535,10 +1716,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="19"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
@@ -1557,10 +1738,10 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="17"/>
+      <c r="B23" s="19"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
@@ -1579,10 +1760,10 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
@@ -1601,10 +1782,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="19"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
@@ -1623,10 +1804,10 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="19"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
@@ -1645,10 +1826,10 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="17"/>
+      <c r="B35" s="19"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
@@ -1667,10 +1848,10 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="21"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
@@ -1689,8 +1870,8 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1716,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,42 +1914,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -1777,172 +1958,172 @@
       <c r="B3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="9" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1957,54 +2138,54 @@
       <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2019,54 +2200,54 @@
       <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2081,54 +2262,54 @@
       <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2143,54 +2324,54 @@
       <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2205,54 +2386,54 @@
       <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2267,54 +2448,54 @@
       <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2329,54 +2510,54 @@
       <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2391,54 +2572,54 @@
       <c r="H32" s="23"/>
     </row>
     <row r="33" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G33" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H33" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2453,131 +2634,137 @@
       <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="G36" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="9" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="22" t="s">
+      <c r="H37" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="A20:H20"/>
@@ -2586,6 +2773,836 @@
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A35:H35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="34"/>
+    </row>
+    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F33" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="34"/>
+    </row>
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A32:H32"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A6:H6"/>
@@ -2596,16 +3613,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>